<commit_message>
lo dejo ya por ahoy, voy con un poco de retraso
</commit_message>
<xml_diff>
--- a/src/test/resources/TemaEntityTestData.xlsx
+++ b/src/test/resources/TemaEntityTestData.xlsx
@@ -19,14 +19,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>INTERSECCION</t>
   </si>
   <si>
-    <t>Deportes</t>
-  </si>
-  <si>
     <t>¿En qué grado sigue usted el fútbol?</t>
   </si>
   <si>
@@ -36,12 +33,6 @@
     <t>¿Considera que las chapas debe ser deporte olímpico?</t>
   </si>
   <si>
-    <t>Política</t>
-  </si>
-  <si>
-    <t>Sociedad</t>
-  </si>
-  <si>
     <t>¿Le gusta la natación?</t>
   </si>
   <si>
@@ -70,6 +61,36 @@
   </si>
   <si>
     <t>PREGUNTA_ENTRADA</t>
+  </si>
+  <si>
+    <t>Tema1</t>
+  </si>
+  <si>
+    <t>Tema2</t>
+  </si>
+  <si>
+    <t>Tema3</t>
+  </si>
+  <si>
+    <t>Tema4</t>
+  </si>
+  <si>
+    <t>Tema5</t>
+  </si>
+  <si>
+    <t>Tema6</t>
+  </si>
+  <si>
+    <t>Tema7</t>
+  </si>
+  <si>
+    <t>Tema8</t>
+  </si>
+  <si>
+    <t>Tema9</t>
+  </si>
+  <si>
+    <t>Tema10</t>
   </si>
 </sst>
 </file>
@@ -431,7 +452,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -442,7 +463,7 @@
   <dimension ref="B1:R12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B12"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,13 +506,13 @@
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -509,14 +530,14 @@
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
         <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
       </c>
       <c r="D3" s="3" t="str">
         <f t="shared" ref="D3:D12" si="0">CONCATENATE("{",B3,",",C3,"}")</f>
-        <v>{Deportes,¿En qué grado sigue usted el fútbol?}</v>
+        <v>{Tema1,¿En qué grado sigue usted el fútbol?}</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
@@ -531,14 +552,14 @@
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D4" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>{Deportes,¿Le gusta el automovilismo?}</v>
+        <v>{Tema2,¿Le gusta el automovilismo?}</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
@@ -553,14 +574,14 @@
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>{Deportes,¿Considera que las chapas debe ser deporte olímpico?}</v>
+        <v>{Tema3,¿Considera que las chapas debe ser deporte olímpico?}</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -575,14 +596,14 @@
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D6" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>{Deportes,¿Le gusta la natación?}</v>
+        <v>{Tema4,¿Le gusta la natación?}</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
@@ -597,14 +618,14 @@
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D7" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>{Deportes,¿Le gusta el baloncesto?}</v>
+        <v>{Tema5,¿Le gusta el baloncesto?}</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -619,14 +640,14 @@
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D8" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>{Deportes,¿Práctica golf?}</v>
+        <v>{Tema6,¿Práctica golf?}</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
@@ -641,56 +662,56 @@
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D9" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>{Política,¿Qúe nota pone a nuestros políticas?}</v>
+        <v>{Tema7,¿Qúe nota pone a nuestros políticas?}</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D10" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>{Política,¿Está de acuerdo con los partidos que nos representan?}</v>
+        <v>{Tema8,¿Está de acuerdo con los partidos que nos representan?}</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D11" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>{Política,¿Crees en los políticos?}</v>
+        <v>{Tema9,¿Crees en los políticos?}</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D12" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>{Sociedad,¿Cómo valora la situación laboral en España?}</v>
+        <v>{Tema10,¿Cómo valora la situación laboral en España?}</v>
       </c>
     </row>
   </sheetData>

</xml_diff>